<commit_message>
add render domain to ALLOWED_HOSTS
</commit_message>
<xml_diff>
--- a/2025 VN defense organization-Final-Vn.xlsx
+++ b/2025 VN defense organization-Final-Vn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tn/Documents/vnw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBF74BE-A681-C348-92DA-BE13AE9794B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98DF7AD4-3B8B-4C41-9C0B-2E2C1E91098E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7260" yWindow="3100" windowWidth="37540" windowHeight="18700" xr2:uid="{2CAD3706-C0EC-48C6-84C8-39C682C8A411}"/>
+    <workbookView xWindow="10500" yWindow="4500" windowWidth="37540" windowHeight="18700" xr2:uid="{2CAD3706-C0EC-48C6-84C8-39C682C8A411}"/>
   </bookViews>
   <sheets>
     <sheet name="organizations" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -139,12 +139,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Sáp nhập Cục Bản đồ và Cục Tác chiến, tổ chức lại thành Cục Tác chiến; 
-https://xaydungchinhsach.chinhphu.vn/sap-nhap-to-chuc-lai-cac-co-quan-thuoc-bo-quoc-phong-bo-tong-tham-muu-tong-cuc-chinh-tri-119250305200345134.htm</t>
+          <t xml:space="preserve">Sáp nhập Cục Bản đồ và Cục Tác chiến, tổ chức lại thành Cục Tác chiến; 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>https://xaydungchinhsach.chinhphu.vn/sap-nhap-to-chuc-lai-cac-co-quan-thuoc-bo-quoc-phong-bo-tong-tham-muu-tong-cuc-chinh-tri-119250305200345134.htm</t>
         </r>
       </text>
     </comment>
@@ -14907,7 +14916,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -15004,6 +15013,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -15050,7 +15065,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -15076,9 +15091,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -15089,6 +15101,10 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -15427,8 +15443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E7E2AB-7E28-44DA-9181-773026E98B79}">
   <dimension ref="A1:W3172"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+    <sheetView tabSelected="1" topLeftCell="B108" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44:E171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15457,7 +15473,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
@@ -15527,12 +15543,12 @@
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
@@ -15555,12 +15571,12 @@
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D9" t="s">
@@ -15589,7 +15605,7 @@
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>4</v>
       </c>
       <c r="E11" t="s">
@@ -15786,18 +15802,23 @@
       </c>
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D44" t="s">
+      <c r="D44" s="20" t="s">
         <v>50</v>
       </c>
+      <c r="E44" s="20"/>
       <c r="F44" t="s">
         <v>2697</v>
       </c>
     </row>
+    <row r="45" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+    </row>
     <row r="46" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D46" t="s">
+      <c r="D46" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="20" t="s">
         <v>2737</v>
       </c>
       <c r="F46" t="s">
@@ -15814,24 +15835,32 @@
       </c>
     </row>
     <row r="47" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E47" t="s">
+      <c r="D47" s="20"/>
+      <c r="E47" s="20" t="s">
         <v>2738</v>
       </c>
     </row>
     <row r="48" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E48" t="s">
+      <c r="D48" s="20"/>
+      <c r="E48" s="20" t="s">
         <v>2735</v>
       </c>
     </row>
     <row r="49" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="E49" t="s">
+      <c r="D49" s="20"/>
+      <c r="E49" s="20" t="s">
         <v>2736</v>
       </c>
     </row>
+    <row r="50" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+    </row>
     <row r="51" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D51" t="s">
+      <c r="D51" s="20" t="s">
         <v>52</v>
       </c>
+      <c r="E51" s="20"/>
       <c r="F51" t="s">
         <v>2699</v>
       </c>
@@ -15852,147 +15881,187 @@
       </c>
     </row>
     <row r="52" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="E52" t="s">
+      <c r="D52" s="20"/>
+      <c r="E52" s="20" t="s">
         <v>2449</v>
       </c>
     </row>
     <row r="53" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="E53" t="s">
+      <c r="D53" s="20"/>
+      <c r="E53" s="20" t="s">
         <v>2748</v>
       </c>
     </row>
     <row r="54" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="E54" t="s">
+      <c r="D54" s="20"/>
+      <c r="E54" s="20" t="s">
         <v>2749</v>
       </c>
     </row>
     <row r="55" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="E55" t="s">
+      <c r="D55" s="20"/>
+      <c r="E55" s="20" t="s">
         <v>2750</v>
       </c>
     </row>
     <row r="56" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="E56" t="s">
+      <c r="D56" s="20"/>
+      <c r="E56" s="20" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="57" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="E57" t="s">
+      <c r="D57" s="20"/>
+      <c r="E57" s="20" t="s">
         <v>2751</v>
       </c>
     </row>
     <row r="58" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="E58" t="s">
+      <c r="D58" s="20"/>
+      <c r="E58" s="20" t="s">
         <v>2752</v>
       </c>
     </row>
     <row r="59" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="E59" t="s">
+      <c r="D59" s="20"/>
+      <c r="E59" s="20" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="60" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="E60" t="s">
+      <c r="D60" s="20"/>
+      <c r="E60" s="20" t="s">
         <v>1347</v>
       </c>
     </row>
     <row r="61" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="E61" t="s">
+      <c r="D61" s="20"/>
+      <c r="E61" s="20" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="62" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="E62" t="s">
+      <c r="D62" s="20"/>
+      <c r="E62" s="20" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="63" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="E63" t="s">
+      <c r="D63" s="20"/>
+      <c r="E63" s="20" t="s">
         <v>2753</v>
       </c>
     </row>
+    <row r="64" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D64" s="20"/>
+      <c r="E64" s="20"/>
+    </row>
+    <row r="65" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D65" s="20"/>
+      <c r="E65" s="20"/>
+    </row>
     <row r="66" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D66" t="s">
+      <c r="D66" s="20" t="s">
         <v>53</v>
       </c>
+      <c r="E66" s="20"/>
       <c r="F66" t="s">
         <v>2701</v>
       </c>
     </row>
     <row r="67" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E67" t="s">
+      <c r="D67" s="20"/>
+      <c r="E67" s="20" t="s">
         <v>888</v>
       </c>
     </row>
     <row r="68" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E68" t="s">
+      <c r="D68" s="20"/>
+      <c r="E68" s="20" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="69" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E69" t="s">
+      <c r="D69" s="20"/>
+      <c r="E69" s="20" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="70" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E70" t="s">
+      <c r="D70" s="20"/>
+      <c r="E70" s="20" t="s">
         <v>889</v>
       </c>
     </row>
     <row r="71" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E71" t="s">
+      <c r="D71" s="20"/>
+      <c r="E71" s="20" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="72" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E72" t="s">
+      <c r="D72" s="20"/>
+      <c r="E72" s="20" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="73" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E73" t="s">
+      <c r="D73" s="20"/>
+      <c r="E73" s="20" t="s">
         <v>2754</v>
       </c>
     </row>
     <row r="74" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E74" t="s">
+      <c r="D74" s="20"/>
+      <c r="E74" s="20" t="s">
         <v>2755</v>
       </c>
     </row>
     <row r="75" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E75" t="s">
+      <c r="D75" s="20"/>
+      <c r="E75" s="20" t="s">
         <v>2756</v>
       </c>
     </row>
     <row r="76" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E76" t="s">
+      <c r="D76" s="20"/>
+      <c r="E76" s="20" t="s">
         <v>2757</v>
       </c>
     </row>
     <row r="77" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E77" t="s">
+      <c r="D77" s="20"/>
+      <c r="E77" s="20" t="s">
         <v>2758</v>
       </c>
     </row>
     <row r="78" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E78" t="s">
+      <c r="D78" s="20"/>
+      <c r="E78" s="20" t="s">
         <v>2759</v>
       </c>
     </row>
     <row r="79" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E79" t="s">
+      <c r="D79" s="20"/>
+      <c r="E79" s="20" t="s">
         <v>2760</v>
       </c>
     </row>
     <row r="80" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E80" t="s">
+      <c r="D80" s="20"/>
+      <c r="E80" s="20" t="s">
         <v>2761</v>
       </c>
     </row>
+    <row r="81" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D81" s="20"/>
+      <c r="E81" s="20"/>
+    </row>
     <row r="82" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D82" t="s">
+      <c r="D82" s="20" t="s">
         <v>48</v>
       </c>
+      <c r="E82" s="20"/>
       <c r="F82" t="s">
         <v>2703</v>
       </c>
@@ -16007,60 +16076,75 @@
       </c>
     </row>
     <row r="83" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E83" s="11" t="s">
+      <c r="D83" s="20"/>
+      <c r="E83" s="21" t="s">
         <v>2707</v>
       </c>
     </row>
     <row r="84" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E84" s="11" t="s">
+      <c r="D84" s="20"/>
+      <c r="E84" s="21" t="s">
         <v>2708</v>
       </c>
     </row>
     <row r="85" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E85" s="11" t="s">
+      <c r="D85" s="20"/>
+      <c r="E85" s="21" t="s">
         <v>2709</v>
       </c>
     </row>
     <row r="86" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E86" s="11" t="s">
+      <c r="D86" s="20"/>
+      <c r="E86" s="21" t="s">
         <v>2710</v>
       </c>
     </row>
     <row r="87" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E87" s="11" t="s">
+      <c r="D87" s="20"/>
+      <c r="E87" s="21" t="s">
         <v>2711</v>
       </c>
     </row>
     <row r="88" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E88" s="11" t="s">
+      <c r="D88" s="20"/>
+      <c r="E88" s="21" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="89" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E89" s="11" t="s">
+      <c r="D89" s="20"/>
+      <c r="E89" s="21" t="s">
         <v>2040</v>
       </c>
     </row>
     <row r="90" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E90" s="11" t="s">
+      <c r="D90" s="20"/>
+      <c r="E90" s="21" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="91" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E91" s="11"/>
+      <c r="D91" s="20"/>
+      <c r="E91" s="21"/>
     </row>
     <row r="92" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D92" t="s">
+      <c r="D92" s="20" t="s">
         <v>49</v>
       </c>
+      <c r="E92" s="20"/>
       <c r="F92" t="s">
         <v>2763</v>
       </c>
     </row>
+    <row r="93" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D93" s="20"/>
+      <c r="E93" s="20"/>
+    </row>
     <row r="94" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D94" t="s">
+      <c r="D94" s="20" t="s">
         <v>54</v>
       </c>
+      <c r="E94" s="20"/>
       <c r="F94" t="s">
         <v>2773</v>
       </c>
@@ -16078,49 +16162,62 @@
       </c>
     </row>
     <row r="95" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E95" t="s">
+      <c r="D95" s="20"/>
+      <c r="E95" s="20" t="s">
         <v>2707</v>
       </c>
     </row>
     <row r="96" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E96" t="s">
+      <c r="D96" s="20"/>
+      <c r="E96" s="20" t="s">
         <v>2769</v>
       </c>
     </row>
     <row r="97" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E97" t="s">
+      <c r="D97" s="20"/>
+      <c r="E97" s="20" t="s">
         <v>2770</v>
       </c>
     </row>
     <row r="98" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E98" t="s">
+      <c r="D98" s="20"/>
+      <c r="E98" s="20" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="99" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E99" t="s">
+      <c r="D99" s="20"/>
+      <c r="E99" s="20" t="s">
         <v>2771</v>
       </c>
     </row>
     <row r="100" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E100" t="s">
+      <c r="D100" s="20"/>
+      <c r="E100" s="20" t="s">
         <v>2772</v>
       </c>
     </row>
     <row r="101" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E101" t="s">
+      <c r="D101" s="20"/>
+      <c r="E101" s="20" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="102" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E102" t="s">
+      <c r="D102" s="20"/>
+      <c r="E102" s="20" t="s">
         <v>614</v>
       </c>
     </row>
+    <row r="103" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D103" s="20"/>
+      <c r="E103" s="20"/>
+    </row>
     <row r="104" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D104" t="s">
+      <c r="D104" s="20" t="s">
         <v>2774</v>
       </c>
+      <c r="E104" s="20"/>
       <c r="F104" t="s">
         <v>2778</v>
       </c>
@@ -16135,49 +16232,62 @@
       </c>
     </row>
     <row r="105" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E105" t="s">
+      <c r="D105" s="20"/>
+      <c r="E105" s="20" t="s">
         <v>2792</v>
       </c>
     </row>
     <row r="106" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E106" t="s">
+      <c r="D106" s="20"/>
+      <c r="E106" s="20" t="s">
         <v>2793</v>
       </c>
     </row>
     <row r="107" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E107" t="s">
+      <c r="D107" s="20"/>
+      <c r="E107" s="20" t="s">
         <v>2794</v>
       </c>
     </row>
     <row r="108" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E108" t="s">
+      <c r="D108" s="20"/>
+      <c r="E108" s="20" t="s">
         <v>2795</v>
       </c>
     </row>
     <row r="109" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E109" t="s">
+      <c r="D109" s="20"/>
+      <c r="E109" s="20" t="s">
         <v>2796</v>
       </c>
     </row>
     <row r="110" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E110" t="s">
+      <c r="D110" s="20"/>
+      <c r="E110" s="20" t="s">
         <v>2797</v>
       </c>
     </row>
     <row r="111" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E111" t="s">
+      <c r="D111" s="20"/>
+      <c r="E111" s="20" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="112" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E112" t="s">
+      <c r="D112" s="20"/>
+      <c r="E112" s="20" t="s">
         <v>614</v>
       </c>
     </row>
+    <row r="113" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D113" s="20"/>
+      <c r="E113" s="20"/>
+    </row>
     <row r="114" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D114" t="s">
+      <c r="D114" s="20" t="s">
         <v>55</v>
       </c>
+      <c r="E114" s="20"/>
       <c r="F114" t="s">
         <v>2799</v>
       </c>
@@ -16192,84 +16302,104 @@
       </c>
     </row>
     <row r="115" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E115" t="s">
+      <c r="D115" s="20"/>
+      <c r="E115" s="20" t="s">
         <v>2803</v>
       </c>
     </row>
     <row r="116" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E116" t="s">
+      <c r="D116" s="20"/>
+      <c r="E116" s="20" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="117" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E117" t="s">
+      <c r="D117" s="20"/>
+      <c r="E117" s="20" t="s">
         <v>2804</v>
       </c>
     </row>
     <row r="118" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E118" t="s">
+      <c r="D118" s="20"/>
+      <c r="E118" s="20" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="119" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E119" t="s">
+      <c r="D119" s="20"/>
+      <c r="E119" s="20" t="s">
         <v>1594</v>
       </c>
     </row>
     <row r="120" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E120" t="s">
+      <c r="D120" s="20"/>
+      <c r="E120" s="20" t="s">
         <v>2805</v>
       </c>
     </row>
     <row r="121" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E121" t="s">
+      <c r="D121" s="20"/>
+      <c r="E121" s="20" t="s">
         <v>2806</v>
       </c>
     </row>
     <row r="122" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E122" t="s">
+      <c r="D122" s="20"/>
+      <c r="E122" s="20" t="s">
         <v>2807</v>
       </c>
     </row>
     <row r="123" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E123" t="s">
+      <c r="D123" s="20"/>
+      <c r="E123" s="20" t="s">
         <v>2808</v>
       </c>
     </row>
     <row r="124" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E124" t="s">
+      <c r="D124" s="20"/>
+      <c r="E124" s="20" t="s">
         <v>2814</v>
       </c>
     </row>
     <row r="125" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E125" t="s">
+      <c r="D125" s="20"/>
+      <c r="E125" s="20" t="s">
         <v>2809</v>
       </c>
     </row>
     <row r="126" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E126" t="s">
+      <c r="D126" s="20"/>
+      <c r="E126" s="20" t="s">
         <v>2810</v>
       </c>
     </row>
     <row r="127" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E127" t="s">
+      <c r="D127" s="20"/>
+      <c r="E127" s="20" t="s">
         <v>2811</v>
       </c>
     </row>
     <row r="128" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E128" t="s">
+      <c r="D128" s="20"/>
+      <c r="E128" s="20" t="s">
         <v>2812</v>
       </c>
     </row>
     <row r="129" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E129" t="s">
+      <c r="D129" s="20"/>
+      <c r="E129" s="20" t="s">
         <v>2813</v>
       </c>
     </row>
+    <row r="130" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D130" s="20"/>
+      <c r="E130" s="20"/>
+    </row>
     <row r="131" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D131" t="s">
+      <c r="D131" s="20" t="s">
         <v>56</v>
       </c>
+      <c r="E131" s="20"/>
       <c r="F131" t="s">
         <v>2816</v>
       </c>
@@ -16287,7 +16417,8 @@
       </c>
     </row>
     <row r="132" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E132" t="s">
+      <c r="D132" s="20"/>
+      <c r="E132" s="20" t="s">
         <v>2821</v>
       </c>
       <c r="F132" t="s">
@@ -16297,8 +16428,13 @@
         <v>2823</v>
       </c>
     </row>
+    <row r="133" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D133" s="20"/>
+      <c r="E133" s="20"/>
+    </row>
     <row r="134" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E134" t="s">
+      <c r="D134" s="20"/>
+      <c r="E134" s="20" t="s">
         <v>19</v>
       </c>
       <c r="F134" t="s">
@@ -16309,7 +16445,8 @@
       </c>
     </row>
     <row r="135" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E135" t="s">
+      <c r="D135" s="20"/>
+      <c r="E135" s="20" t="s">
         <v>287</v>
       </c>
       <c r="F135" t="s">
@@ -16317,7 +16454,8 @@
       </c>
     </row>
     <row r="136" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E136" t="s">
+      <c r="D136" s="20"/>
+      <c r="E136" s="20" t="s">
         <v>2827</v>
       </c>
       <c r="G136" t="s">
@@ -16325,7 +16463,8 @@
       </c>
     </row>
     <row r="137" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E137" t="s">
+      <c r="D137" s="20"/>
+      <c r="E137" s="20" t="s">
         <v>2803</v>
       </c>
       <c r="F137" t="s">
@@ -16336,7 +16475,8 @@
       </c>
     </row>
     <row r="138" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E138" t="s">
+      <c r="D138" s="20"/>
+      <c r="E138" s="20" t="s">
         <v>350</v>
       </c>
       <c r="F138" t="s">
@@ -16347,7 +16487,8 @@
       </c>
     </row>
     <row r="139" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E139" t="s">
+      <c r="D139" s="20"/>
+      <c r="E139" s="20" t="s">
         <v>1531</v>
       </c>
       <c r="F139" t="s">
@@ -16358,7 +16499,8 @@
       </c>
     </row>
     <row r="140" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E140" t="s">
+      <c r="D140" s="20"/>
+      <c r="E140" s="20" t="s">
         <v>913</v>
       </c>
       <c r="F140" t="s">
@@ -16366,7 +16508,8 @@
       </c>
     </row>
     <row r="141" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E141" t="s">
+      <c r="D141" s="20"/>
+      <c r="E141" s="20" t="s">
         <v>2836</v>
       </c>
       <c r="F141" t="s">
@@ -16377,7 +16520,8 @@
       </c>
     </row>
     <row r="142" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E142" t="s">
+      <c r="D142" s="20"/>
+      <c r="E142" s="20" t="s">
         <v>93</v>
       </c>
       <c r="F142" t="s">
@@ -16388,7 +16532,8 @@
       </c>
     </row>
     <row r="143" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E143" t="s">
+      <c r="D143" s="20"/>
+      <c r="E143" s="20" t="s">
         <v>1402</v>
       </c>
       <c r="F143" t="s">
@@ -16396,15 +16541,21 @@
       </c>
     </row>
     <row r="144" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E144" t="s">
+      <c r="D144" s="20"/>
+      <c r="E144" s="20" t="s">
         <v>2842</v>
       </c>
       <c r="F144" t="s">
         <v>2843</v>
       </c>
     </row>
-    <row r="146" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E146" t="s">
+    <row r="145" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D145" s="20"/>
+      <c r="E145" s="20"/>
+    </row>
+    <row r="146" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D146" s="20"/>
+      <c r="E146" s="20" t="s">
         <v>2851</v>
       </c>
       <c r="F146" t="s">
@@ -16420,8 +16571,9 @@
         <v>2855</v>
       </c>
     </row>
-    <row r="147" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E147" t="s">
+    <row r="147" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D147" s="20"/>
+      <c r="E147" s="20" t="s">
         <v>2857</v>
       </c>
       <c r="F147" t="s">
@@ -16434,8 +16586,9 @@
         <v>2860</v>
       </c>
     </row>
-    <row r="148" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E148" t="s">
+    <row r="148" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D148" s="20"/>
+      <c r="E148" s="20" t="s">
         <v>2861</v>
       </c>
       <c r="F148" t="s">
@@ -16448,8 +16601,9 @@
         <v>2863</v>
       </c>
     </row>
-    <row r="149" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E149" t="s">
+    <row r="149" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D149" s="20"/>
+      <c r="E149" s="20" t="s">
         <v>2864</v>
       </c>
       <c r="F149" t="s">
@@ -16468,8 +16622,9 @@
         <v>2867</v>
       </c>
     </row>
-    <row r="150" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E150" t="s">
+    <row r="150" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D150" s="20"/>
+      <c r="E150" s="20" t="s">
         <v>2870</v>
       </c>
       <c r="F150" t="s">
@@ -16485,8 +16640,9 @@
         <v>2874</v>
       </c>
     </row>
-    <row r="151" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E151" t="s">
+    <row r="151" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D151" s="20"/>
+      <c r="E151" s="20" t="s">
         <v>2875</v>
       </c>
       <c r="F151" t="s">
@@ -16502,8 +16658,9 @@
         <v>2877</v>
       </c>
     </row>
-    <row r="152" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E152" t="s">
+    <row r="152" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D152" s="20"/>
+      <c r="E152" s="20" t="s">
         <v>2879</v>
       </c>
       <c r="F152" t="s">
@@ -16513,8 +16670,9 @@
         <v>2880</v>
       </c>
     </row>
-    <row r="153" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E153" t="s">
+    <row r="153" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D153" s="20"/>
+      <c r="E153" s="20" t="s">
         <v>2882</v>
       </c>
       <c r="F153" t="s">
@@ -16524,8 +16682,9 @@
         <v>2846</v>
       </c>
     </row>
-    <row r="154" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E154" t="s">
+    <row r="154" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D154" s="20"/>
+      <c r="E154" s="20" t="s">
         <v>2884</v>
       </c>
       <c r="F154" t="s">
@@ -16535,8 +16694,9 @@
         <v>2847</v>
       </c>
     </row>
-    <row r="155" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E155" t="s">
+    <row r="155" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D155" s="20"/>
+      <c r="E155" s="20" t="s">
         <v>2886</v>
       </c>
       <c r="F155" t="s">
@@ -16549,8 +16709,9 @@
         <v>2891</v>
       </c>
     </row>
-    <row r="156" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E156" t="s">
+    <row r="156" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D156" s="20"/>
+      <c r="E156" s="20" t="s">
         <v>2887</v>
       </c>
       <c r="F156" t="s">
@@ -16563,16 +16724,22 @@
         <v>2892</v>
       </c>
     </row>
-    <row r="157" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E157" t="s">
+    <row r="157" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D157" s="20"/>
+      <c r="E157" s="20" t="s">
         <v>2888</v>
       </c>
       <c r="F157" t="s">
         <v>2850</v>
       </c>
     </row>
-    <row r="159" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E159" t="s">
+    <row r="158" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D158" s="20"/>
+      <c r="E158" s="20"/>
+    </row>
+    <row r="159" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D159" s="20"/>
+      <c r="E159" s="20" t="s">
         <v>2898</v>
       </c>
       <c r="F159" t="s">
@@ -16582,8 +16749,9 @@
         <v>2894</v>
       </c>
     </row>
-    <row r="160" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E160" t="s">
+    <row r="160" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D160" s="20"/>
+      <c r="E160" s="20" t="s">
         <v>2899</v>
       </c>
       <c r="F160" t="s">
@@ -16591,7 +16759,8 @@
       </c>
     </row>
     <row r="161" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="E161" t="s">
+      <c r="D161" s="20"/>
+      <c r="E161" s="20" t="s">
         <v>2900</v>
       </c>
       <c r="F161" t="s">
@@ -16601,10 +16770,15 @@
         <v>2897</v>
       </c>
     </row>
+    <row r="162" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="D162" s="20"/>
+      <c r="E162" s="20"/>
+    </row>
     <row r="163" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D163" t="s">
+      <c r="D163" s="20" t="s">
         <v>57</v>
       </c>
+      <c r="E163" s="20"/>
       <c r="F163" t="s">
         <v>2901</v>
       </c>
@@ -16612,10 +16786,15 @@
         <v>2902</v>
       </c>
     </row>
+    <row r="164" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="D164" s="20"/>
+      <c r="E164" s="20"/>
+    </row>
     <row r="165" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D165" t="s">
+      <c r="D165" s="20" t="s">
         <v>58</v>
       </c>
+      <c r="E165" s="20"/>
       <c r="F165" t="s">
         <v>2903</v>
       </c>
@@ -16632,23 +16811,38 @@
         <v>2907</v>
       </c>
     </row>
+    <row r="166" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="D166" s="20"/>
+      <c r="E166" s="20"/>
+    </row>
     <row r="167" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D167" t="s">
+      <c r="D167" s="20" t="s">
         <v>59</v>
       </c>
+      <c r="E167" s="20"/>
     </row>
     <row r="168" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D168" t="s">
+      <c r="D168" s="20" t="s">
         <v>60</v>
       </c>
+      <c r="E168" s="20"/>
     </row>
     <row r="169" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D169" t="s">
+      <c r="D169" s="20" t="s">
         <v>61</v>
       </c>
+      <c r="E169" s="20"/>
+    </row>
+    <row r="170" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="D170" s="20"/>
+      <c r="E170" s="20"/>
+    </row>
+    <row r="171" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="D171" s="20"/>
+      <c r="E171" s="20"/>
     </row>
     <row r="173" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C173" s="17" t="s">
+      <c r="C173" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F173" t="s">
@@ -17080,7 +17274,7 @@
       </c>
     </row>
     <row r="245" spans="4:16" x14ac:dyDescent="0.2">
-      <c r="D245" s="19" t="s">
+      <c r="D245" s="18" t="s">
         <v>27</v>
       </c>
       <c r="F245" t="s">
@@ -17480,7 +17674,7 @@
       </c>
     </row>
     <row r="300" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C300" s="17" t="s">
+      <c r="C300" s="16" t="s">
         <v>6</v>
       </c>
       <c r="F300" t="s">
@@ -17491,7 +17685,7 @@
       </c>
     </row>
     <row r="306" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C306" s="17" t="s">
+      <c r="C306" s="16" t="s">
         <v>7</v>
       </c>
       <c r="F306" t="s">
@@ -17702,7 +17896,7 @@
       </c>
     </row>
     <row r="340" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C340" s="17" t="s">
+      <c r="C340" s="16" t="s">
         <v>8</v>
       </c>
       <c r="F340" t="s">
@@ -18200,7 +18394,7 @@
       </c>
     </row>
     <row r="417" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C417" s="16" t="s">
+      <c r="C417" s="15" t="s">
         <v>14</v>
       </c>
       <c r="F417" t="s">
@@ -18272,7 +18466,7 @@
       </c>
     </row>
     <row r="430" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C430" s="17" t="s">
+      <c r="C430" s="16" t="s">
         <v>10</v>
       </c>
       <c r="F430" t="s">
@@ -18355,7 +18549,7 @@
       </c>
     </row>
     <row r="447" spans="3:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="C447" s="17" t="s">
+      <c r="C447" s="16" t="s">
         <v>9</v>
       </c>
       <c r="F447" s="5" t="s">
@@ -18430,7 +18624,7 @@
       </c>
     </row>
     <row r="460" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C460" s="17" t="s">
+      <c r="C460" s="16" t="s">
         <v>11</v>
       </c>
       <c r="F460" t="s">
@@ -18517,7 +18711,7 @@
       </c>
     </row>
     <row r="476" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C476" s="17" t="s">
+      <c r="C476" s="16" t="s">
         <v>12</v>
       </c>
       <c r="F476" t="s">
@@ -18634,7 +18828,7 @@
       </c>
     </row>
     <row r="499" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C499" s="17" t="s">
+      <c r="C499" s="16" t="s">
         <v>13</v>
       </c>
       <c r="F499" t="s">
@@ -18675,7 +18869,7 @@
       </c>
     </row>
     <row r="507" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C507" s="17" t="s">
+      <c r="C507" s="16" t="s">
         <v>15</v>
       </c>
       <c r="F507" t="s">
@@ -18733,7 +18927,7 @@
       </c>
     </row>
     <row r="516" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C516" s="17" t="s">
+      <c r="C516" s="16" t="s">
         <v>16</v>
       </c>
       <c r="F516" t="s">
@@ -18877,7 +19071,7 @@
       </c>
     </row>
     <row r="535" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C535" s="17" t="s">
+      <c r="C535" s="16" t="s">
         <v>17</v>
       </c>
       <c r="F535" t="s">
@@ -18942,7 +19136,7 @@
       </c>
     </row>
     <row r="546" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C546" s="17" t="s">
+      <c r="C546" s="16" t="s">
         <v>18</v>
       </c>
       <c r="F546" t="s">
@@ -18984,12 +19178,12 @@
       </c>
     </row>
     <row r="554" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C554" s="17" t="s">
+      <c r="C554" s="16" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="555" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="D555" s="17" t="s">
+      <c r="D555" s="16" t="s">
         <v>149</v>
       </c>
       <c r="G555" t="s">
@@ -19085,7 +19279,7 @@
       </c>
     </row>
     <row r="574" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D574" s="17" t="s">
+      <c r="D574" s="16" t="s">
         <v>131</v>
       </c>
     </row>
@@ -19362,7 +19556,7 @@
       </c>
     </row>
     <row r="628" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D628" s="17" t="s">
+      <c r="D628" s="16" t="s">
         <v>132</v>
       </c>
       <c r="G628" t="s">
@@ -19846,7 +20040,7 @@
       </c>
     </row>
     <row r="712" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D712" s="17" t="s">
+      <c r="D712" s="16" t="s">
         <v>133</v>
       </c>
       <c r="G712" t="s">
@@ -20197,7 +20391,7 @@
       </c>
     </row>
     <row r="780" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D780" s="17" t="s">
+      <c r="D780" s="16" t="s">
         <v>135</v>
       </c>
       <c r="G780" t="s">
@@ -21003,7 +21197,7 @@
       </c>
     </row>
     <row r="885" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D885" s="17" t="s">
+      <c r="D885" s="16" t="s">
         <v>136</v>
       </c>
       <c r="G885" t="s">
@@ -21600,7 +21794,7 @@
       </c>
     </row>
     <row r="979" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D979" s="17" t="s">
+      <c r="D979" s="16" t="s">
         <v>137</v>
       </c>
       <c r="G979" s="6" t="s">
@@ -22143,7 +22337,7 @@
       </c>
     </row>
     <row r="1075" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D1075" s="17" t="s">
+      <c r="D1075" s="16" t="s">
         <v>138</v>
       </c>
       <c r="G1075" s="6" t="s">
@@ -22604,7 +22798,7 @@
       </c>
     </row>
     <row r="1148" spans="3:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="C1148" s="17" t="s">
+      <c r="C1148" s="16" t="s">
         <v>139</v>
       </c>
       <c r="F1148" t="s">
@@ -22993,7 +23187,7 @@
       </c>
     </row>
     <row r="1219" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C1219" s="17" t="s">
+      <c r="C1219" s="16" t="s">
         <v>140</v>
       </c>
       <c r="F1219" t="s">
@@ -23388,12 +23582,12 @@
       </c>
     </row>
     <row r="1288" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C1288" s="17" t="s">
+      <c r="C1288" s="16" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="1289" spans="3:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="D1289" s="17" t="s">
+      <c r="D1289" s="16" t="s">
         <v>150</v>
       </c>
       <c r="G1289" s="8" t="s">
@@ -23513,7 +23707,7 @@
       </c>
     </row>
     <row r="1312" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D1312" s="17" t="s">
+      <c r="D1312" s="16" t="s">
         <v>1170</v>
       </c>
       <c r="G1312" t="s">
@@ -23943,7 +24137,7 @@
       </c>
     </row>
     <row r="1398" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D1398" s="17" t="s">
+      <c r="D1398" s="16" t="s">
         <v>1231</v>
       </c>
       <c r="G1398" t="s">
@@ -24053,7 +24247,7 @@
       </c>
     </row>
     <row r="1419" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D1419" s="17" t="s">
+      <c r="D1419" s="16" t="s">
         <v>1247</v>
       </c>
       <c r="G1419" t="s">
@@ -24216,7 +24410,7 @@
       </c>
     </row>
     <row r="1450" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D1450" s="17" t="s">
+      <c r="D1450" s="16" t="s">
         <v>1270</v>
       </c>
       <c r="G1450" t="s">
@@ -24339,7 +24533,7 @@
       </c>
     </row>
     <row r="1473" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D1473" s="17" t="s">
+      <c r="D1473" s="16" t="s">
         <v>1288</v>
       </c>
       <c r="G1473" t="s">
@@ -24481,12 +24675,12 @@
       </c>
     </row>
     <row r="1500" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C1500" s="17" t="s">
+      <c r="C1500" s="16" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="1501" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D1501" s="17" t="s">
+      <c r="D1501" s="16" t="s">
         <v>145</v>
       </c>
       <c r="G1501" t="s">
@@ -25796,7 +25990,7 @@
       <c r="E1730" t="s">
         <v>1580</v>
       </c>
-      <c r="G1730" s="18" t="s">
+      <c r="G1730" s="17" t="s">
         <v>3774</v>
       </c>
       <c r="H1730" t="s">
@@ -25825,187 +26019,187 @@
       <c r="F1731" t="s">
         <v>1619</v>
       </c>
-      <c r="R1731" s="13"/>
+      <c r="R1731" s="12"/>
     </row>
     <row r="1732" spans="5:18" x14ac:dyDescent="0.2">
       <c r="F1732" t="s">
         <v>1587</v>
       </c>
-      <c r="R1732" s="13"/>
+      <c r="R1732" s="12"/>
     </row>
     <row r="1733" spans="5:18" x14ac:dyDescent="0.2">
       <c r="F1733" t="s">
         <v>350</v>
       </c>
-      <c r="R1733" s="13"/>
+      <c r="R1733" s="12"/>
     </row>
     <row r="1734" spans="5:18" x14ac:dyDescent="0.2">
       <c r="F1734" t="s">
         <v>351</v>
       </c>
-      <c r="R1734" s="13"/>
+      <c r="R1734" s="12"/>
     </row>
     <row r="1735" spans="5:18" x14ac:dyDescent="0.2">
       <c r="F1735" t="s">
         <v>1588</v>
       </c>
-      <c r="R1735" s="13"/>
+      <c r="R1735" s="12"/>
     </row>
     <row r="1736" spans="5:18" x14ac:dyDescent="0.2">
       <c r="F1736" t="s">
         <v>1589</v>
       </c>
-      <c r="R1736" s="13"/>
+      <c r="R1736" s="12"/>
     </row>
     <row r="1737" spans="5:18" x14ac:dyDescent="0.2">
       <c r="F1737" t="s">
         <v>1590</v>
       </c>
-      <c r="R1737" s="13"/>
+      <c r="R1737" s="12"/>
     </row>
     <row r="1738" spans="5:18" x14ac:dyDescent="0.2">
       <c r="F1738" t="s">
         <v>1591</v>
       </c>
-      <c r="R1738" s="13"/>
+      <c r="R1738" s="12"/>
     </row>
     <row r="1739" spans="5:18" x14ac:dyDescent="0.2">
       <c r="F1739" t="s">
         <v>1592</v>
       </c>
-      <c r="R1739" s="13"/>
+      <c r="R1739" s="12"/>
     </row>
     <row r="1740" spans="5:18" x14ac:dyDescent="0.2">
       <c r="F1740" t="s">
         <v>1593</v>
       </c>
-      <c r="R1740" s="13"/>
+      <c r="R1740" s="12"/>
     </row>
     <row r="1741" spans="5:18" x14ac:dyDescent="0.2">
       <c r="F1741" t="s">
         <v>888</v>
       </c>
-      <c r="R1741" s="13"/>
+      <c r="R1741" s="12"/>
     </row>
     <row r="1742" spans="5:18" x14ac:dyDescent="0.2">
       <c r="F1742" t="s">
         <v>1594</v>
       </c>
-      <c r="R1742" s="13"/>
+      <c r="R1742" s="12"/>
     </row>
     <row r="1743" spans="5:18" x14ac:dyDescent="0.2">
       <c r="F1743" t="s">
         <v>1595</v>
       </c>
-      <c r="R1743" s="13"/>
+      <c r="R1743" s="12"/>
     </row>
     <row r="1744" spans="5:18" x14ac:dyDescent="0.2">
       <c r="F1744" t="s">
         <v>1596</v>
       </c>
-      <c r="R1744" s="13"/>
+      <c r="R1744" s="12"/>
     </row>
     <row r="1745" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F1745" t="s">
         <v>1597</v>
       </c>
-      <c r="R1745" s="13"/>
+      <c r="R1745" s="12"/>
     </row>
     <row r="1746" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F1746" t="s">
         <v>1598</v>
       </c>
-      <c r="R1746" s="13"/>
+      <c r="R1746" s="12"/>
     </row>
     <row r="1747" spans="6:18" x14ac:dyDescent="0.2">
-      <c r="R1747" s="13"/>
+      <c r="R1747" s="12"/>
     </row>
     <row r="1748" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F1748" t="s">
         <v>3792</v>
       </c>
-      <c r="R1748" s="13"/>
+      <c r="R1748" s="12"/>
     </row>
     <row r="1749" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F1749" t="s">
         <v>3787</v>
       </c>
-      <c r="R1749" s="13"/>
+      <c r="R1749" s="12"/>
     </row>
     <row r="1750" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F1750" t="s">
         <v>3780</v>
       </c>
-      <c r="R1750" s="13"/>
+      <c r="R1750" s="12"/>
     </row>
     <row r="1751" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F1751" t="s">
         <v>3797</v>
       </c>
-      <c r="R1751" s="13"/>
+      <c r="R1751" s="12"/>
     </row>
     <row r="1752" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F1752" t="s">
         <v>1601</v>
       </c>
-      <c r="R1752" s="13"/>
+      <c r="R1752" s="12"/>
     </row>
     <row r="1753" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F1753" t="s">
         <v>3802</v>
       </c>
-      <c r="R1753" s="13"/>
+      <c r="R1753" s="12"/>
     </row>
     <row r="1754" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F1754" t="s">
         <v>3803</v>
       </c>
-      <c r="R1754" s="13"/>
+      <c r="R1754" s="12"/>
     </row>
     <row r="1755" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F1755" t="s">
         <v>3800</v>
       </c>
-      <c r="R1755" s="13"/>
+      <c r="R1755" s="12"/>
     </row>
     <row r="1756" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F1756" t="s">
         <v>3794</v>
       </c>
-      <c r="R1756" s="13"/>
+      <c r="R1756" s="12"/>
     </row>
     <row r="1757" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F1757" t="s">
         <v>3868</v>
       </c>
-      <c r="R1757" s="13"/>
+      <c r="R1757" s="12"/>
     </row>
     <row r="1758" spans="6:18" x14ac:dyDescent="0.2">
-      <c r="R1758" s="13"/>
+      <c r="R1758" s="12"/>
     </row>
     <row r="1759" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F1759" t="s">
         <v>1602</v>
       </c>
-      <c r="R1759" s="13"/>
+      <c r="R1759" s="12"/>
     </row>
     <row r="1760" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F1760" t="s">
         <v>1603</v>
       </c>
-      <c r="R1760" s="13"/>
+      <c r="R1760" s="12"/>
     </row>
     <row r="1761" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F1761" t="s">
         <v>3779</v>
       </c>
-      <c r="R1761" s="13"/>
+      <c r="R1761" s="12"/>
     </row>
     <row r="1762" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F1762" t="s">
         <v>3791</v>
       </c>
-      <c r="R1762" s="13"/>
+      <c r="R1762" s="12"/>
     </row>
     <row r="1763" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F1763" t="s">
@@ -26216,7 +26410,7 @@
       <c r="E1807" t="s">
         <v>3755</v>
       </c>
-      <c r="H1807" s="13" t="s">
+      <c r="H1807" s="12" t="s">
         <v>1634</v>
       </c>
     </row>
@@ -26240,7 +26434,7 @@
       </c>
     </row>
     <row r="1814" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D1814" s="17" t="s">
+      <c r="D1814" s="16" t="s">
         <v>144</v>
       </c>
       <c r="G1814" t="s">
@@ -26633,7 +26827,7 @@
       </c>
     </row>
     <row r="1852" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D1852" s="17" t="s">
+      <c r="D1852" s="16" t="s">
         <v>143</v>
       </c>
       <c r="G1852" t="s">
@@ -27345,7 +27539,7 @@
       </c>
     </row>
     <row r="1921" spans="4:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="D1921" s="17" t="s">
+      <c r="D1921" s="16" t="s">
         <v>146</v>
       </c>
       <c r="G1921" t="s">
@@ -27797,7 +27991,7 @@
       </c>
     </row>
     <row r="1994" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D1994" s="17" t="s">
+      <c r="D1994" s="16" t="s">
         <v>147</v>
       </c>
       <c r="G1994" t="s">
@@ -28015,7 +28209,7 @@
       </c>
     </row>
     <row r="2037" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D2037" s="17" t="s">
+      <c r="D2037" s="16" t="s">
         <v>148</v>
       </c>
       <c r="G2037" t="s">
@@ -28097,12 +28291,12 @@
       </c>
     </row>
     <row r="2056" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B2056" s="17" t="s">
+      <c r="B2056" s="16" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="2057" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C2057" s="17" t="s">
+      <c r="C2057" s="16" t="s">
         <v>152</v>
       </c>
       <c r="F2057" t="s">
@@ -28254,7 +28448,7 @@
       </c>
     </row>
     <row r="2082" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C2082" s="17" t="s">
+      <c r="C2082" s="16" t="s">
         <v>153</v>
       </c>
       <c r="F2082" t="s">
@@ -28455,7 +28649,7 @@
       </c>
     </row>
     <row r="2126" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C2126" s="17" t="s">
+      <c r="C2126" s="16" t="s">
         <v>692</v>
       </c>
       <c r="F2126" t="s">
@@ -28645,7 +28839,7 @@
       </c>
     </row>
     <row r="2165" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C2165" s="17" t="s">
+      <c r="C2165" s="16" t="s">
         <v>154</v>
       </c>
       <c r="F2165" t="s">
@@ -28829,7 +29023,7 @@
       </c>
     </row>
     <row r="2201" spans="3:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="C2201" s="17" t="s">
+      <c r="C2201" s="16" t="s">
         <v>155</v>
       </c>
       <c r="F2201" s="8" t="s">
@@ -29007,7 +29201,7 @@
       </c>
     </row>
     <row r="2237" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C2237" s="17" t="s">
+      <c r="C2237" s="16" t="s">
         <v>2211</v>
       </c>
       <c r="E2237" t="s">
@@ -29404,7 +29598,7 @@
       </c>
     </row>
     <row r="2291" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C2291" s="17" t="s">
+      <c r="C2291" s="16" t="s">
         <v>2303</v>
       </c>
       <c r="F2291" t="s">
@@ -29430,7 +29624,7 @@
       </c>
     </row>
     <row r="2293" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C2293" s="17" t="s">
+      <c r="C2293" s="16" t="s">
         <v>2304</v>
       </c>
       <c r="F2293" t="s">
@@ -29758,7 +29952,7 @@
       </c>
     </row>
     <row r="2340" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C2340" s="17" t="s">
+      <c r="C2340" s="16" t="s">
         <v>2371</v>
       </c>
       <c r="E2340" t="s">
@@ -29969,7 +30163,7 @@
       </c>
     </row>
     <row r="2381" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C2381" s="17" t="s">
+      <c r="C2381" s="16" t="s">
         <v>156</v>
       </c>
       <c r="F2381" t="s">
@@ -30197,12 +30391,12 @@
       </c>
     </row>
     <row r="2426" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B2426" s="17" t="s">
+      <c r="B2426" s="16" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="2427" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C2427" s="17" t="s">
+      <c r="C2427" s="16" t="s">
         <v>685</v>
       </c>
       <c r="E2427" t="s">
@@ -30315,7 +30509,7 @@
       </c>
     </row>
     <row r="2448" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C2448" s="17" t="s">
+      <c r="C2448" s="16" t="s">
         <v>158</v>
       </c>
       <c r="E2448" s="4" t="s">
@@ -30351,7 +30545,7 @@
       </c>
     </row>
     <row r="2455" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C2455" s="17" t="s">
+      <c r="C2455" s="16" t="s">
         <v>159</v>
       </c>
       <c r="E2455" t="s">
@@ -30461,12 +30655,12 @@
       </c>
     </row>
     <row r="2477" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2477" s="17" t="s">
+      <c r="B2477" s="16" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="2478" spans="2:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2478" s="17" t="s">
+      <c r="C2478" s="16" t="s">
         <v>165</v>
       </c>
       <c r="E2478" s="4" t="s">
@@ -31052,7 +31246,7 @@
       </c>
     </row>
     <row r="2597" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C2597" s="17" t="s">
+      <c r="C2597" s="16" t="s">
         <v>166</v>
       </c>
       <c r="F2597" t="s">
@@ -31198,15 +31392,15 @@
       <c r="E2618" s="4" t="s">
         <v>2601</v>
       </c>
-      <c r="G2618" s="20"/>
-      <c r="I2618" s="20"/>
+      <c r="G2618" s="19"/>
+      <c r="I2618" s="19"/>
     </row>
     <row r="2619" spans="4:9" x14ac:dyDescent="0.2">
       <c r="E2619" s="4" t="s">
         <v>2602</v>
       </c>
-      <c r="G2619" s="20"/>
-      <c r="I2619" s="20"/>
+      <c r="G2619" s="19"/>
+      <c r="I2619" s="19"/>
     </row>
     <row r="2620" spans="4:9" x14ac:dyDescent="0.2">
       <c r="E2620" s="4" t="s">
@@ -31326,12 +31520,12 @@
       </c>
     </row>
     <row r="2637" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E2637" s="20" t="s">
+      <c r="E2637" s="19" t="s">
         <v>2621</v>
       </c>
     </row>
     <row r="2638" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E2638" s="20"/>
+      <c r="E2638" s="19"/>
     </row>
     <row r="2639" spans="4:10" x14ac:dyDescent="0.2">
       <c r="E2639" s="4" t="s">
@@ -31394,12 +31588,12 @@
       </c>
     </row>
     <row r="2652" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E2652" s="20" t="s">
+      <c r="E2652" s="19" t="s">
         <v>2633</v>
       </c>
     </row>
     <row r="2653" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E2653" s="20"/>
+      <c r="E2653" s="19"/>
     </row>
     <row r="2654" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E2654" s="4" t="s">
@@ -31442,7 +31636,7 @@
       </c>
     </row>
     <row r="2663" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C2663" s="17" t="s">
+      <c r="C2663" s="16" t="s">
         <v>167</v>
       </c>
       <c r="F2663" t="s">
@@ -31681,7 +31875,7 @@
       </c>
     </row>
     <row r="2707" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2707" s="17" t="s">
+      <c r="B2707" s="16" t="s">
         <v>192</v>
       </c>
     </row>
@@ -31910,7 +32104,7 @@
       </c>
     </row>
     <row r="2737" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B2737" s="17" t="s">
+      <c r="B2737" s="16" t="s">
         <v>178</v>
       </c>
     </row>
@@ -34033,7 +34227,7 @@
       <c r="C3107" t="s">
         <v>284</v>
       </c>
-      <c r="F3107" s="13" t="s">
+      <c r="F3107" s="12" t="s">
         <v>3752</v>
       </c>
     </row>
@@ -34041,7 +34235,7 @@
       <c r="C3109" t="s">
         <v>3753</v>
       </c>
-      <c r="F3109" s="13" t="s">
+      <c r="F3109" s="12" t="s">
         <v>3766</v>
       </c>
     </row>
@@ -34049,7 +34243,7 @@
       <c r="C3111" t="s">
         <v>3754</v>
       </c>
-      <c r="F3111" s="13" t="s">
+      <c r="F3111" s="12" t="s">
         <v>3768</v>
       </c>
     </row>
@@ -34057,7 +34251,7 @@
       <c r="C3113" t="s">
         <v>3756</v>
       </c>
-      <c r="F3113" s="13" t="s">
+      <c r="F3113" s="12" t="s">
         <v>3770</v>
       </c>
     </row>
@@ -34065,32 +34259,32 @@
       <c r="C3115" t="s">
         <v>3757</v>
       </c>
-      <c r="F3115" s="13" t="s">
+      <c r="F3115" s="12" t="s">
         <v>3772</v>
       </c>
     </row>
     <row r="3150" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="F3150" s="13"/>
+      <c r="F3150" s="12"/>
     </row>
     <row r="3151" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C3151" t="s">
         <v>3758</v>
       </c>
-      <c r="F3151" s="13" t="s">
+      <c r="F3151" s="12" t="s">
         <v>3806</v>
       </c>
     </row>
     <row r="3152" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="F3152" s="13"/>
+      <c r="F3152" s="12"/>
     </row>
     <row r="3153" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C3153" t="s">
         <v>3759</v>
       </c>
-      <c r="F3153" s="13"/>
+      <c r="F3153" s="12"/>
     </row>
     <row r="3154" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="F3154" s="13"/>
+      <c r="F3154" s="12"/>
     </row>
     <row r="3155" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C3155" t="s">
@@ -35338,52 +35532,52 @@
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A274" s="12" t="s">
+      <c r="A274" s="11" t="s">
         <v>2780</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A275" s="12" t="s">
+      <c r="A275" s="11" t="s">
         <v>2781</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A276" s="12" t="s">
+      <c r="A276" s="11" t="s">
         <v>2782</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A277" s="12" t="s">
+      <c r="A277" s="11" t="s">
         <v>2783</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A278" s="12" t="s">
+      <c r="A278" s="11" t="s">
         <v>2784</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A279" s="12" t="s">
+      <c r="A279" s="11" t="s">
         <v>2785</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A280" s="12" t="s">
+      <c r="A280" s="11" t="s">
         <v>2786</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A281" s="12" t="s">
+      <c r="A281" s="11" t="s">
         <v>2787</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A282" s="12" t="s">
+      <c r="A282" s="11" t="s">
         <v>2788</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A283" s="12" t="s">
+      <c r="A283" s="11" t="s">
         <v>2789</v>
       </c>
     </row>

</xml_diff>